<commit_message>
after 4th video - installing react js and creating an hello world app - in reacttut/awesomeapp
</commit_message>
<xml_diff>
--- a/Logs.xlsx
+++ b/Logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeevan A. Sawalkar\Desktop\Self Study\00 React js\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C24D89-77A5-4FAD-9273-D9F6A18168C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB155CA-D4C9-41BB-865A-36675B44267F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Sr no</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vs code extensions to be installed. </t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>installing react js</t>
   </si>
 </sst>
 </file>
@@ -374,7 +383,7 @@
   <dimension ref="B3:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,6 +414,9 @@
       <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
@@ -418,10 +430,22 @@
       <c r="B6" s="2">
         <v>3</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>